<commit_message>
Comment Screen #1:   + Frame Search Screen #1:   + Frame Profile Screen #1:   + Frame
</commit_message>
<xml_diff>
--- a/localize/localize.xlsx
+++ b/localize/localize.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="438">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -1304,6 +1304,36 @@
   </si>
   <si>
     <t xml:space="preserve">Follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_followed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã theo dõi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Followed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bình luận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm địa chỉ…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search</t>
   </si>
 </sst>
 </file>
@@ -1500,10 +1530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
+      <selection pane="topLeft" activeCell="C158" activeCellId="0" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3135,6 +3165,50 @@
         <v>427</v>
       </c>
     </row>
+    <row r="155" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Comment #1:   + Fixed data   + New Comment   + Load More Search #1:   + Frame
</commit_message>
<xml_diff>
--- a/localize/localize.xlsx
+++ b/localize/localize.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="447">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -1309,6 +1309,15 @@
     <t xml:space="preserve">lang_follow</t>
   </si>
   <si>
+    <t xml:space="preserve">lang_unfollow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bỏ theo dõi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfollow</t>
+  </si>
+  <si>
     <t xml:space="preserve">lang_followed</t>
   </si>
   <si>
@@ -1334,6 +1343,24 @@
   </si>
   <si>
     <t xml:space="preserve">Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên tài khoản</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang_viewMore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xem thêm…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View more…</t>
   </si>
 </sst>
 </file>
@@ -1530,10 +1557,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C158" activeCellId="0" sqref="C158"/>
+      <selection pane="topLeft" activeCell="A161" activeCellId="0" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3209,6 +3236,39 @@
         <v>437</v>
       </c>
     </row>
+    <row r="159" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>